<commit_message>
created the quarterly figures data preparation and merge with prices
</commit_message>
<xml_diff>
--- a/code/imputationExperiment/results_forecasting_prices_and_returns.xlsx
+++ b/code/imputationExperiment/results_forecasting_prices_and_returns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maarten\Desktop\Afstuderen\thesis_stock_prediction_repo\code\imputationExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED26F8F6-8407-4F18-BD44-91FA0497AECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA0B152-F1C3-438C-8296-7D90F7B34895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results_forecasting_prices" sheetId="2" r:id="rId1"/>
@@ -278,12 +278,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -292,6 +286,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC78F473-F578-42E0-804F-76BE96EAA9B2}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,14 +1158,14 @@
       <c r="E2" s="4"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27" t="s">
+      <c r="J2" s="25"/>
+      <c r="K2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="26"/>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1203,7 +1203,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="8">
@@ -1218,10 +1218,10 @@
       <c r="E4" s="8">
         <v>6.9289662839359233E-3</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="8">
@@ -1238,7 +1238,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="9">
@@ -1253,8 +1253,8 @@
       <c r="E5" s="9">
         <v>9.6275353232265597E-3</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="24" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="9">
@@ -1271,7 +1271,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="9">
@@ -1286,8 +1286,8 @@
       <c r="E6" s="9">
         <v>4.9700916238027753E-3</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="24" t="s">
+      <c r="G6" s="26"/>
+      <c r="H6" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="9">
@@ -1304,7 +1304,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="9">
@@ -1319,8 +1319,8 @@
       <c r="E7" s="9">
         <v>3.6796465916911418E-3</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="24" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="23" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="9">
@@ -1337,7 +1337,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="9">
@@ -1352,8 +1352,8 @@
       <c r="E8" s="9">
         <v>7.6873006038450176E-3</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="24" t="s">
+      <c r="G8" s="26"/>
+      <c r="H8" s="23" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="9">
@@ -1370,7 +1370,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="10">
@@ -1385,8 +1385,8 @@
       <c r="E9" s="10">
         <v>3.5844016789664868E-3</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="24" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="9">
@@ -1403,10 +1403,10 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="9">
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G11" s="25"/>
-      <c r="H11" s="24" t="s">
+      <c r="G11" s="26"/>
+      <c r="H11" s="23" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="9">
@@ -1441,8 +1441,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G12" s="25"/>
-      <c r="H12" s="24" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="9">
@@ -1459,8 +1459,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G13" s="25"/>
-      <c r="H13" s="24" t="s">
+      <c r="G13" s="26"/>
+      <c r="H13" s="23" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="9">
@@ -1477,8 +1477,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G14" s="25"/>
-      <c r="H14" s="24" t="s">
+      <c r="G14" s="26"/>
+      <c r="H14" s="23" t="s">
         <v>7</v>
       </c>
       <c r="I14" s="9">
@@ -1495,8 +1495,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G15" s="25"/>
-      <c r="H15" s="24" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="23" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="9">
@@ -1513,10 +1513,10 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="23" t="s">
         <v>3</v>
       </c>
       <c r="I16" s="9">
@@ -1533,8 +1533,8 @@
       </c>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G17" s="25"/>
-      <c r="H17" s="24" t="s">
+      <c r="G17" s="26"/>
+      <c r="H17" s="23" t="s">
         <v>4</v>
       </c>
       <c r="I17" s="9">
@@ -1551,8 +1551,8 @@
       </c>
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G18" s="25"/>
-      <c r="H18" s="24" t="s">
+      <c r="G18" s="26"/>
+      <c r="H18" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I18" s="9">
@@ -1569,8 +1569,8 @@
       </c>
     </row>
     <row r="19" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G19" s="25"/>
-      <c r="H19" s="24" t="s">
+      <c r="G19" s="26"/>
+      <c r="H19" s="23" t="s">
         <v>6</v>
       </c>
       <c r="I19" s="9">
@@ -1587,8 +1587,8 @@
       </c>
     </row>
     <row r="20" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G20" s="25"/>
-      <c r="H20" s="24" t="s">
+      <c r="G20" s="26"/>
+      <c r="H20" s="23" t="s">
         <v>7</v>
       </c>
       <c r="I20" s="9">
@@ -1605,8 +1605,8 @@
       </c>
     </row>
     <row r="21" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G21" s="25"/>
-      <c r="H21" s="24" t="s">
+      <c r="G21" s="26"/>
+      <c r="H21" s="23" t="s">
         <v>8</v>
       </c>
       <c r="I21" s="10">
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,7 +1755,7 @@
       <c r="E4" s="6">
         <v>9.6654302819582441E-3</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="27" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="19" t="s">
@@ -1790,7 +1790,7 @@
       <c r="E5" s="6">
         <v>6.3619902325711044E-3</v>
       </c>
-      <c r="G5" s="23"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="19" t="s">
         <v>4</v>
       </c>
@@ -1823,7 +1823,7 @@
       <c r="E6" s="6">
         <v>1.2904860388740809E-2</v>
       </c>
-      <c r="G6" s="23"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="19" t="s">
         <v>5</v>
       </c>
@@ -1856,7 +1856,7 @@
       <c r="E7" s="6">
         <v>7.4444054857529442E-3</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="19" t="s">
         <v>6</v>
       </c>
@@ -1889,7 +1889,7 @@
       <c r="E8" s="6">
         <v>8.0810288281656841E-3</v>
       </c>
-      <c r="G8" s="23"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="19" t="s">
         <v>7</v>
       </c>
@@ -1922,7 +1922,7 @@
       <c r="E9" s="7">
         <v>8.7685685960721908E-3</v>
       </c>
-      <c r="G9" s="23"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="19" t="s">
         <v>8</v>
       </c>
@@ -1940,7 +1940,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="27" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="19" t="s">
@@ -1960,7 +1960,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G11" s="23"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="19" t="s">
         <v>4</v>
       </c>
@@ -1978,7 +1978,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G12" s="23"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="19" t="s">
         <v>5</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="G13" s="23"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="19" t="s">
         <v>6</v>
       </c>
@@ -2022,7 +2022,7 @@
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="19" t="s">
         <v>7</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="B15" s="13"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="G15" s="23"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="19" t="s">
         <v>8</v>
       </c>
@@ -2066,7 +2066,7 @@
       <c r="B16" s="13"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="27" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="19" t="s">
@@ -2090,7 +2090,7 @@
       <c r="B17" s="13"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="19" t="s">
         <v>4</v>
       </c>
@@ -2112,7 +2112,7 @@
       <c r="B18" s="13"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="19" t="s">
         <v>5</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="B19" s="13"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="19" t="s">
         <v>6</v>
       </c>
@@ -2156,7 +2156,7 @@
       <c r="B20" s="13"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="19" t="s">
         <v>7</v>
       </c>
@@ -2178,7 +2178,7 @@
       <c r="B21" s="13"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="19" t="s">
         <v>8</v>
       </c>

</xml_diff>